<commit_message>
Finishes the UI portion of the work
</commit_message>
<xml_diff>
--- a/test/resc/bad_tests/654.xlsx
+++ b/test/resc/bad_tests/654.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalto\Documents\VS Code\project-timesaver\test\resc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalto\Documents\VS Code\project-timesaver\test\resc\bad_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22994A8-BB0C-4C64-A2A7-877C47915F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23687576-AE83-4596-819F-475632E53B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39690" yWindow="1410" windowWidth="16200" windowHeight="9480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pay" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2774" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2773" uniqueCount="423">
   <si>
     <t>LEAVE BLANK LEAVE BLANK LEAVE BLANK</t>
   </si>
@@ -1298,9 +1298,6 @@
   </si>
   <si>
     <t>FIRE SERVICE CASUALITIES</t>
-  </si>
-  <si>
-    <t>2021/12/34</t>
   </si>
 </sst>
 </file>
@@ -1336,8 +1333,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2213,11 +2211,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2239,8 +2240,8 @@
       <c r="C3" t="s">
         <v>112</v>
       </c>
-      <c r="D3" t="s">
-        <v>423</v>
+      <c r="D3" s="1">
+        <v>44561</v>
       </c>
       <c r="E3" t="s">
         <v>114</v>

</xml_diff>